<commit_message>
Beginning class 15, some of homework 1
</commit_message>
<xml_diff>
--- a/roster.xlsx
+++ b/roster.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e2603e9ea7112e0/Documents/john-carroll/data1220/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{1329647E-D695-488E-BB86-2E5BA0CCA8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBA7F7B2-8A80-467F-BC6A-EAD1D6D70AC1}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{1329647E-D695-488E-BB86-2E5BA0CCA8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58238C11-C684-404E-92C6-40B249A5DAD9}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1707143D-380A-43BE-A061-61F455F9E1D7}"/>
   </bookViews>
@@ -311,10 +311,10 @@
     <t>title IX issue, extra accomodations</t>
   </si>
   <si>
-    <t>early warning</t>
-  </si>
-  <si>
     <t>SAS accomodations</t>
+  </si>
+  <si>
+    <t>withdrew, early warning</t>
   </si>
 </sst>
 </file>
@@ -378,6 +378,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -699,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CD1E61-1736-4862-91AA-720006710BFD}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection sqref="A1:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -770,7 +774,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -817,7 +821,7 @@
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -974,7 +978,7 @@
         <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1054,7 +1058,7 @@
         <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
homework 4 in progress
</commit_message>
<xml_diff>
--- a/roster.xlsx
+++ b/roster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e2603e9ea7112e0/Documents/john-carroll/data1220/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{1329647E-D695-488E-BB86-2E5BA0CCA8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58238C11-C684-404E-92C6-40B249A5DAD9}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{1329647E-D695-488E-BB86-2E5BA0CCA8FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32CF3539-0813-475C-A318-B6B8B2E24CBD}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1707143D-380A-43BE-A061-61F455F9E1D7}"/>
   </bookViews>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CD1E61-1736-4862-91AA-720006710BFD}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:D30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1080,18 +1080,18 @@
     <hyperlink ref="C16" r:id="rId15" xr:uid="{431DCDA6-5EF6-4F0E-8E29-32288DEFCD4E}"/>
     <hyperlink ref="C17" r:id="rId16" xr:uid="{7D9B57C4-E9B6-4991-BF95-2B73CC3A3614}"/>
     <hyperlink ref="C18" r:id="rId17" xr:uid="{F7CD7DE5-7D16-4C43-B3DA-5842F6E9A145}"/>
-    <hyperlink ref="C19" r:id="rId18" xr:uid="{F8BB29FE-CDAC-459B-8F6F-EB79CB6E8641}"/>
-    <hyperlink ref="C20" r:id="rId19" xr:uid="{BE9777B7-FD67-4FE7-83D2-3C5303CB2757}"/>
-    <hyperlink ref="C21" r:id="rId20" xr:uid="{5DB8DC78-9A1C-484D-97F8-A57F69108D9A}"/>
-    <hyperlink ref="C22" r:id="rId21" xr:uid="{F4E5F495-23B4-4CA9-99CE-13445F51EC56}"/>
-    <hyperlink ref="C23" r:id="rId22" xr:uid="{35A57744-8F31-4CA4-942F-E277A79D0D8E}"/>
-    <hyperlink ref="C24" r:id="rId23" xr:uid="{AD37F5F9-31F8-47C5-BEEF-7D888497B017}"/>
-    <hyperlink ref="C25" r:id="rId24" xr:uid="{CB669E20-6AF0-48B4-97BF-6865E93D2634}"/>
-    <hyperlink ref="C26" r:id="rId25" xr:uid="{C30207E9-6BE8-4E52-A2D1-D24E7CBD3755}"/>
-    <hyperlink ref="C27" r:id="rId26" xr:uid="{7AC042D3-BB00-4A27-8520-64145A98CF64}"/>
-    <hyperlink ref="C28" r:id="rId27" xr:uid="{B26E46DF-8BD0-4152-9137-7F51D5463A13}"/>
-    <hyperlink ref="C29" r:id="rId28" xr:uid="{F03FC487-6A30-44CD-A669-7DA5ED60E01F}"/>
-    <hyperlink ref="C30" r:id="rId29" xr:uid="{7D1EC207-A5A6-4658-8F37-EDFAA1CBAD63}"/>
+    <hyperlink ref="C20" r:id="rId18" xr:uid="{BE9777B7-FD67-4FE7-83D2-3C5303CB2757}"/>
+    <hyperlink ref="C21" r:id="rId19" xr:uid="{5DB8DC78-9A1C-484D-97F8-A57F69108D9A}"/>
+    <hyperlink ref="C22" r:id="rId20" xr:uid="{F4E5F495-23B4-4CA9-99CE-13445F51EC56}"/>
+    <hyperlink ref="C23" r:id="rId21" xr:uid="{35A57744-8F31-4CA4-942F-E277A79D0D8E}"/>
+    <hyperlink ref="C24" r:id="rId22" xr:uid="{AD37F5F9-31F8-47C5-BEEF-7D888497B017}"/>
+    <hyperlink ref="C25" r:id="rId23" xr:uid="{CB669E20-6AF0-48B4-97BF-6865E93D2634}"/>
+    <hyperlink ref="C26" r:id="rId24" xr:uid="{C30207E9-6BE8-4E52-A2D1-D24E7CBD3755}"/>
+    <hyperlink ref="C27" r:id="rId25" xr:uid="{7AC042D3-BB00-4A27-8520-64145A98CF64}"/>
+    <hyperlink ref="C28" r:id="rId26" xr:uid="{B26E46DF-8BD0-4152-9137-7F51D5463A13}"/>
+    <hyperlink ref="C29" r:id="rId27" xr:uid="{F03FC487-6A30-44CD-A669-7DA5ED60E01F}"/>
+    <hyperlink ref="C30" r:id="rId28" xr:uid="{7D1EC207-A5A6-4658-8F37-EDFAA1CBAD63}"/>
+    <hyperlink ref="C19" r:id="rId29" xr:uid="{F8BB29FE-CDAC-459B-8F6F-EB79CB6E8641}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>